<commit_message>
all chnges till now
</commit_message>
<xml_diff>
--- a/WebApplication1/Template/MyDataTemplate.xlsx
+++ b/WebApplication1/Template/MyDataTemplate.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\esahu\source\repos\OpenXMLExcel\WebApplication1\Template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D19DFE48-0F71-4AA4-9291-2BE2085BD929}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{286D3960-3A0B-42E4-904C-634D819BE33A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,13 +17,17 @@
     <sheet name="Database &amp; Connectivity" sheetId="2" r:id="rId2"/>
     <sheet name="Power Systems" sheetId="3" r:id="rId3"/>
     <sheet name="Z Systems" sheetId="4" r:id="rId4"/>
+    <sheet name="Product Count" sheetId="6" r:id="rId5"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'Product Count'!$A$1:$K$1</definedName>
+  </definedNames>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="18">
   <si>
     <t>Product Hierarchy</t>
   </si>
@@ -60,6 +64,32 @@
   </si>
   <si>
     <t>Z Systems</t>
+  </si>
+  <si>
+    <t>Engineer Owner</t>
+  </si>
+  <si>
+    <t>Family Owner</t>
+  </si>
+  <si>
+    <t>Finance Owner</t>
+  </si>
+  <si>
+    <t>Pcode 
+Count</t>
+  </si>
+  <si>
+    <t>Active 
+SKU 
+Count</t>
+  </si>
+  <si>
+    <t>Inactive 
+SKU 
+Count</t>
+  </si>
+  <si>
+    <t>BU Owner</t>
   </si>
 </sst>
 </file>
@@ -166,7 +196,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -179,8 +209,14 @@
         <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -188,11 +224,20 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -235,6 +280,15 @@
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -636,11 +690,11 @@
       <c r="Y1" s="8"/>
     </row>
     <row r="2" spans="1:25" ht="22.5" x14ac:dyDescent="0.45">
-      <c r="A2" s="22" t="s">
+      <c r="A2" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="22"/>
-      <c r="C2" s="22"/>
+      <c r="B2" s="25"/>
+      <c r="C2" s="25"/>
       <c r="E2" s="8"/>
       <c r="F2" s="8"/>
       <c r="G2" s="8"/>
@@ -1451,4 +1505,70 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2C63458-CE14-4763-837A-3AF9856D458B}">
+  <dimension ref="A1:K1"/>
+  <sheetViews>
+    <sheetView zoomScale="68" zoomScaleNormal="68" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="12.7265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.7265625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.453125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.81640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.7265625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.90625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.36328125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.08984375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="20.36328125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="18.26953125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="19.26953125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" s="22" customFormat="1" ht="39" x14ac:dyDescent="0.3">
+      <c r="A1" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="23" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="23" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="24" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1" s="24" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1" s="24" t="s">
+        <v>16</v>
+      </c>
+      <c r="H1" s="24" t="s">
+        <v>17</v>
+      </c>
+      <c r="I1" s="24" t="s">
+        <v>11</v>
+      </c>
+      <c r="J1" s="24" t="s">
+        <v>12</v>
+      </c>
+      <c r="K1" s="24" t="s">
+        <v>13</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:K1" xr:uid="{E2C63458-CE14-4763-837A-3AF9856D458B}"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Prod summary page updated
</commit_message>
<xml_diff>
--- a/WebApplication1/Template/MyDataTemplate.xlsx
+++ b/WebApplication1/Template/MyDataTemplate.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\esahu\source\repos\OpenXMLExcel\WebApplication1\Template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33906E74-0C54-4416-900F-C3C6679EBFA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1DDA5EA-17B9-419A-89F4-A44622CBF27B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,14 +20,14 @@
     <sheet name="Product Summary" sheetId="6" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'Product Summary'!$A$1:$O$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'Product Summary'!$A$1:$V$1</definedName>
   </definedNames>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="27">
   <si>
     <t>Product Hierarchy</t>
   </si>
@@ -105,6 +105,31 @@
     <t>Partner
 Inactive 
 SKU Count</t>
+  </si>
+  <si>
+    <t>Tier 1 
+Count</t>
+  </si>
+  <si>
+    <t>Tier 2 
+Count</t>
+  </si>
+  <si>
+    <t>Tier 3 
+Count</t>
+  </si>
+  <si>
+    <t>Tier 4 
+Count</t>
+  </si>
+  <si>
+    <t>Tier 5 
+Count</t>
+  </si>
+  <si>
+    <t>Tier
+(unassigned) 
+Count</t>
   </si>
 </sst>
 </file>
@@ -1524,7 +1549,7 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2C63458-CE14-4763-837A-3AF9856D458B}">
-  <dimension ref="A1:O1"/>
+  <dimension ref="A1:V1"/>
   <sheetViews>
     <sheetView zoomScale="68" zoomScaleNormal="68" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -1539,15 +1564,15 @@
     <col min="4" max="4" width="18.81640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11.7265625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11.90625" bestFit="1" customWidth="1"/>
-    <col min="7" max="10" width="11.90625" customWidth="1"/>
-    <col min="11" max="11" width="13.36328125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="15.08984375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="20.36328125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="18.26953125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="19.26953125" bestFit="1" customWidth="1"/>
+    <col min="7" max="17" width="11.90625" customWidth="1"/>
+    <col min="18" max="18" width="13.36328125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="15.08984375" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="20.36328125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="18.26953125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="19.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" s="22" customFormat="1" ht="39" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:22" s="22" customFormat="1" ht="39" x14ac:dyDescent="0.3">
       <c r="A1" s="23" t="s">
         <v>1</v>
       </c>
@@ -1568,32 +1593,51 @@
       </c>
       <c r="G1" s="24"/>
       <c r="H1" s="24" t="s">
+        <v>21</v>
+      </c>
+      <c r="I1" s="24" t="s">
+        <v>22</v>
+      </c>
+      <c r="J1" s="24" t="s">
+        <v>23</v>
+      </c>
+      <c r="K1" s="24" t="s">
+        <v>24</v>
+      </c>
+      <c r="L1" s="24" t="s">
+        <v>25</v>
+      </c>
+      <c r="M1" s="24" t="s">
+        <v>26</v>
+      </c>
+      <c r="N1" s="24"/>
+      <c r="O1" s="24" t="s">
         <v>17</v>
       </c>
-      <c r="I1" s="24" t="s">
+      <c r="P1" s="24" t="s">
         <v>18</v>
       </c>
-      <c r="J1" s="24" t="s">
+      <c r="Q1" s="24" t="s">
         <v>19</v>
       </c>
-      <c r="K1" s="24" t="s">
+      <c r="R1" s="24" t="s">
         <v>20</v>
       </c>
-      <c r="L1" s="24" t="s">
+      <c r="S1" s="24" t="s">
         <v>15</v>
       </c>
-      <c r="M1" s="24" t="s">
+      <c r="T1" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="N1" s="24" t="s">
+      <c r="U1" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="O1" s="24" t="s">
+      <c r="V1" s="24" t="s">
         <v>13</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:O1" xr:uid="{E2C63458-CE14-4763-837A-3AF9856D458B}"/>
+  <autoFilter ref="A1:V1" xr:uid="{E2C63458-CE14-4763-837A-3AF9856D458B}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Works before filling and formattong page6
</commit_message>
<xml_diff>
--- a/WebApplication1/Template/MyDataTemplate.xlsx
+++ b/WebApplication1/Template/MyDataTemplate.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\esahu\source\repos\OpenXMLExcel\WebApplication1\Template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1DDA5EA-17B9-419A-89F4-A44622CBF27B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7112D317-3D10-420A-8CC2-6FD23625355F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="643" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hierarchy" sheetId="1" r:id="rId1"/>
@@ -18,16 +18,18 @@
     <sheet name="Power Systems" sheetId="3" r:id="rId3"/>
     <sheet name="Z Systems" sheetId="4" r:id="rId4"/>
     <sheet name="Product Summary" sheetId="6" r:id="rId5"/>
+    <sheet name="Tier Summary" sheetId="7" r:id="rId6"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'Product Summary'!$A$1:$V$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">'Tier Summary'!$A$1:$H$1</definedName>
   </definedNames>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="31">
   <si>
     <t>Product Hierarchy</t>
   </si>
@@ -130,6 +132,19 @@
     <t>Tier
 (unassigned) 
 Count</t>
+  </si>
+  <si>
+    <t>Tier</t>
+  </si>
+  <si>
+    <t>Tier
+Description</t>
+  </si>
+  <si>
+    <t>Pcode</t>
+  </si>
+  <si>
+    <t>Pcode Name</t>
   </si>
 </sst>
 </file>
@@ -256,7 +271,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -273,11 +288,48 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -327,6 +379,18 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -730,11 +794,11 @@
       <c r="Y1" s="8"/>
     </row>
     <row r="2" spans="1:25" ht="22.5" x14ac:dyDescent="0.45">
-      <c r="A2" s="25" t="s">
+      <c r="A2" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="25"/>
-      <c r="C2" s="25"/>
+      <c r="B2" s="29"/>
+      <c r="C2" s="29"/>
       <c r="E2" s="8"/>
       <c r="F2" s="8"/>
       <c r="G2" s="8"/>
@@ -1558,18 +1622,20 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="12.7265625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.7265625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.453125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.81640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.7265625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.90625" bestFit="1" customWidth="1"/>
-    <col min="7" max="17" width="11.90625" customWidth="1"/>
-    <col min="18" max="18" width="13.36328125" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="15.08984375" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="20.36328125" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="18.26953125" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="19.26953125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.7265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.6328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.453125" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="12.81640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="5.6328125" customWidth="1"/>
+    <col min="8" max="12" width="12.81640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="18.54296875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="5.6328125" customWidth="1"/>
+    <col min="15" max="18" width="16.6328125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="16.36328125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="21.7265625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="19.6328125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="20.6328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:22" s="22" customFormat="1" ht="39" x14ac:dyDescent="0.3">
@@ -1641,4 +1707,56 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9CFD09F3-1C1E-427B-B616-0A4EB97515DD}">
+  <dimension ref="A1:H1"/>
+  <sheetViews>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="10.08984375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.36328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.7265625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.1796875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.7265625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.7265625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.453125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.81640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" ht="26.5" x14ac:dyDescent="0.35">
+      <c r="A1" s="25" t="s">
+        <v>27</v>
+      </c>
+      <c r="B1" s="26" t="s">
+        <v>28</v>
+      </c>
+      <c r="C1" s="26" t="s">
+        <v>29</v>
+      </c>
+      <c r="D1" s="26" t="s">
+        <v>30</v>
+      </c>
+      <c r="E1" s="27" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" s="27" t="s">
+        <v>2</v>
+      </c>
+      <c r="G1" s="27" t="s">
+        <v>3</v>
+      </c>
+      <c r="H1" s="28" t="s">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:H1" xr:uid="{9CFD09F3-1C1E-427B-B616-0A4EB97515DD}"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Changes till Tier Summary at one place
</commit_message>
<xml_diff>
--- a/WebApplication1/Template/MyDataTemplate.xlsx
+++ b/WebApplication1/Template/MyDataTemplate.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\esahu\source\repos\OpenXMLExcel\WebApplication1\Template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7112D317-3D10-420A-8CC2-6FD23625355F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A6BF43C-AE24-4F56-8BDC-4F33DAD766CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="643" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1713,7 +1713,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9CFD09F3-1C1E-427B-B616-0A4EB97515DD}">
   <dimension ref="A1:H1"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView zoomScale="77" zoomScaleNormal="77" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
necessary changes for 2 separate files in zip
</commit_message>
<xml_diff>
--- a/WebApplication1/Template/MyDataTemplate.xlsx
+++ b/WebApplication1/Template/MyDataTemplate.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\esahu\source\repos\OpenXMLExcel\WebApplication1\Template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A6BF43C-AE24-4F56-8BDC-4F33DAD766CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{221B3E03-ECBC-4013-88FC-FB922988B209}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="643" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -18,18 +18,16 @@
     <sheet name="Power Systems" sheetId="3" r:id="rId3"/>
     <sheet name="Z Systems" sheetId="4" r:id="rId4"/>
     <sheet name="Product Summary" sheetId="6" r:id="rId5"/>
-    <sheet name="Tier Summary" sheetId="7" r:id="rId6"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'Product Summary'!$A$1:$V$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">'Tier Summary'!$A$1:$H$1</definedName>
   </definedNames>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="27">
   <si>
     <t>Product Hierarchy</t>
   </si>
@@ -132,19 +130,6 @@
     <t>Tier
 (unassigned) 
 Count</t>
-  </si>
-  <si>
-    <t>Tier</t>
-  </si>
-  <si>
-    <t>Tier
-Description</t>
-  </si>
-  <si>
-    <t>Pcode</t>
-  </si>
-  <si>
-    <t>Pcode Name</t>
   </si>
 </sst>
 </file>
@@ -271,7 +256,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -288,48 +273,11 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -379,18 +327,6 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -794,11 +730,11 @@
       <c r="Y1" s="8"/>
     </row>
     <row r="2" spans="1:25" ht="22.5" x14ac:dyDescent="0.45">
-      <c r="A2" s="29" t="s">
+      <c r="A2" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="29"/>
-      <c r="C2" s="29"/>
+      <c r="B2" s="25"/>
+      <c r="C2" s="25"/>
       <c r="E2" s="8"/>
       <c r="F2" s="8"/>
       <c r="G2" s="8"/>
@@ -1707,56 +1643,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9CFD09F3-1C1E-427B-B616-0A4EB97515DD}">
-  <dimension ref="A1:H1"/>
-  <sheetViews>
-    <sheetView zoomScale="77" zoomScaleNormal="77" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="10.08984375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.36328125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.7265625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.1796875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.7265625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.7265625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="19.453125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="18.81640625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:8" ht="26.5" x14ac:dyDescent="0.35">
-      <c r="A1" s="25" t="s">
-        <v>27</v>
-      </c>
-      <c r="B1" s="26" t="s">
-        <v>28</v>
-      </c>
-      <c r="C1" s="26" t="s">
-        <v>29</v>
-      </c>
-      <c r="D1" s="26" t="s">
-        <v>30</v>
-      </c>
-      <c r="E1" s="27" t="s">
-        <v>1</v>
-      </c>
-      <c r="F1" s="27" t="s">
-        <v>2</v>
-      </c>
-      <c r="G1" s="27" t="s">
-        <v>3</v>
-      </c>
-      <c r="H1" s="28" t="s">
-        <v>4</v>
-      </c>
-    </row>
-  </sheetData>
-  <autoFilter ref="A1:H1" xr:uid="{9CFD09F3-1C1E-427B-B616-0A4EB97515DD}"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
made prod hierarchy changes for faster
</commit_message>
<xml_diff>
--- a/WebApplication1/Template/MyDataTemplate.xlsx
+++ b/WebApplication1/Template/MyDataTemplate.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24527"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\esahu\source\repos\OpenXMLExcel\WebApplication1\Template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{221B3E03-ECBC-4013-88FC-FB922988B209}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A73119DA-F2F4-4CE4-8736-6085CECD3076}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="643" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,17 +17,14 @@
     <sheet name="Database &amp; Connectivity" sheetId="2" r:id="rId2"/>
     <sheet name="Power Systems" sheetId="3" r:id="rId3"/>
     <sheet name="Z Systems" sheetId="4" r:id="rId4"/>
-    <sheet name="Product Summary" sheetId="6" r:id="rId5"/>
+    <sheet name="Product Summary" sheetId="5" r:id="rId5"/>
   </sheets>
-  <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'Product Summary'!$A$1:$V$1</definedName>
-  </definedNames>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="11">
   <si>
     <t>Product Hierarchy</t>
   </si>
@@ -64,72 +61,6 @@
   </si>
   <si>
     <t>Z Systems</t>
-  </si>
-  <si>
-    <t>Engineer Owner</t>
-  </si>
-  <si>
-    <t>Family Owner</t>
-  </si>
-  <si>
-    <t>Finance Owner</t>
-  </si>
-  <si>
-    <t>Pcode 
-Count</t>
-  </si>
-  <si>
-    <t>BU Owner</t>
-  </si>
-  <si>
-    <t>Total 
-SKU 
-Count</t>
-  </si>
-  <si>
-    <t>Rocket
-Active 
-SKU Count</t>
-  </si>
-  <si>
-    <t>Rocket
-Inactive 
-SKU Count</t>
-  </si>
-  <si>
-    <t>Partner
-Active 
-SKU Count</t>
-  </si>
-  <si>
-    <t>Partner
-Inactive 
-SKU Count</t>
-  </si>
-  <si>
-    <t>Tier 1 
-Count</t>
-  </si>
-  <si>
-    <t>Tier 2 
-Count</t>
-  </si>
-  <si>
-    <t>Tier 3 
-Count</t>
-  </si>
-  <si>
-    <t>Tier 4 
-Count</t>
-  </si>
-  <si>
-    <t>Tier 5 
-Count</t>
-  </si>
-  <si>
-    <t>Tier
-(unassigned) 
-Count</t>
   </si>
 </sst>
 </file>
@@ -236,7 +167,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -249,14 +180,8 @@
         <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -264,20 +189,11 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -320,15 +236,6 @@
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -730,11 +637,11 @@
       <c r="Y1" s="8"/>
     </row>
     <row r="2" spans="1:25" ht="22.5" x14ac:dyDescent="0.45">
-      <c r="A2" s="25" t="s">
+      <c r="A2" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="25"/>
-      <c r="C2" s="25"/>
+      <c r="B2" s="22"/>
+      <c r="C2" s="22"/>
       <c r="E2" s="8"/>
       <c r="F2" s="8"/>
       <c r="G2" s="8"/>
@@ -1548,99 +1455,13 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2C63458-CE14-4763-837A-3AF9856D458B}">
-  <dimension ref="A1:V1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E4CA8D1F-1157-4282-9791-3897C49F83F0}">
+  <dimension ref="A1"/>
   <sheetViews>
-    <sheetView zoomScale="68" zoomScaleNormal="68" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="13.7265625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.6328125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.453125" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="12.81640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="5.6328125" customWidth="1"/>
-    <col min="8" max="12" width="12.81640625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="18.54296875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="5.6328125" customWidth="1"/>
-    <col min="15" max="18" width="16.6328125" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="16.36328125" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="21.7265625" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="19.6328125" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="20.6328125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:22" s="22" customFormat="1" ht="39" x14ac:dyDescent="0.3">
-      <c r="A1" s="23" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" s="23" t="s">
-        <v>2</v>
-      </c>
-      <c r="C1" s="23" t="s">
-        <v>3</v>
-      </c>
-      <c r="D1" s="23" t="s">
-        <v>4</v>
-      </c>
-      <c r="E1" s="24" t="s">
-        <v>14</v>
-      </c>
-      <c r="F1" s="24" t="s">
-        <v>16</v>
-      </c>
-      <c r="G1" s="24"/>
-      <c r="H1" s="24" t="s">
-        <v>21</v>
-      </c>
-      <c r="I1" s="24" t="s">
-        <v>22</v>
-      </c>
-      <c r="J1" s="24" t="s">
-        <v>23</v>
-      </c>
-      <c r="K1" s="24" t="s">
-        <v>24</v>
-      </c>
-      <c r="L1" s="24" t="s">
-        <v>25</v>
-      </c>
-      <c r="M1" s="24" t="s">
-        <v>26</v>
-      </c>
-      <c r="N1" s="24"/>
-      <c r="O1" s="24" t="s">
-        <v>17</v>
-      </c>
-      <c r="P1" s="24" t="s">
-        <v>18</v>
-      </c>
-      <c r="Q1" s="24" t="s">
-        <v>19</v>
-      </c>
-      <c r="R1" s="24" t="s">
-        <v>20</v>
-      </c>
-      <c r="S1" s="24" t="s">
-        <v>15</v>
-      </c>
-      <c r="T1" s="24" t="s">
-        <v>11</v>
-      </c>
-      <c r="U1" s="24" t="s">
-        <v>12</v>
-      </c>
-      <c r="V1" s="24" t="s">
-        <v>13</v>
-      </c>
-    </row>
-  </sheetData>
-  <autoFilter ref="A1:V1" xr:uid="{E2C63458-CE14-4763-837A-3AF9856D458B}"/>
+  <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated BU name changes
</commit_message>
<xml_diff>
--- a/WebApplication1/Template/MyDataTemplate.xlsx
+++ b/WebApplication1/Template/MyDataTemplate.xlsx
@@ -1,30 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\esahu\source\repos\OpenXMLExcel\WebApplication1\Template\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\AppPublish_DownloadExcel_Stage\Template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A73119DA-F2F4-4CE4-8736-6085CECD3076}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89019D7D-68B7-40A8-A8AA-D1FC4BE4B074}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="643" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="740" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hierarchy" sheetId="1" r:id="rId1"/>
-    <sheet name="Database &amp; Connectivity" sheetId="2" r:id="rId2"/>
-    <sheet name="Power Systems" sheetId="3" r:id="rId3"/>
-    <sheet name="Z Systems" sheetId="4" r:id="rId4"/>
-    <sheet name="Product Summary" sheetId="5" r:id="rId5"/>
+    <sheet name="Application Modernization" sheetId="2" r:id="rId2"/>
+    <sheet name="Data Modernization" sheetId="3" r:id="rId3"/>
+    <sheet name="Infrastructure Modernization" sheetId="4" r:id="rId4"/>
+    <sheet name="Product Summary" sheetId="6" r:id="rId5"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'Product Summary'!$A$1:$V$1</definedName>
+  </definedNames>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="27">
   <si>
     <t>Product Hierarchy</t>
   </si>
@@ -54,13 +57,79 @@
     <t>Finance Manager</t>
   </si>
   <si>
-    <t>Database &amp; Connectivity</t>
-  </si>
-  <si>
-    <t>Power Systems</t>
-  </si>
-  <si>
-    <t>Z Systems</t>
+    <t>Engineer Owner</t>
+  </si>
+  <si>
+    <t>Family Owner</t>
+  </si>
+  <si>
+    <t>Finance Owner</t>
+  </si>
+  <si>
+    <t>Pcode 
+Count</t>
+  </si>
+  <si>
+    <t>BU Owner</t>
+  </si>
+  <si>
+    <t>Total 
+SKU 
+Count</t>
+  </si>
+  <si>
+    <t>Rocket
+Active 
+SKU Count</t>
+  </si>
+  <si>
+    <t>Rocket
+Inactive 
+SKU Count</t>
+  </si>
+  <si>
+    <t>Partner
+Active 
+SKU Count</t>
+  </si>
+  <si>
+    <t>Partner
+Inactive 
+SKU Count</t>
+  </si>
+  <si>
+    <t>Tier 1 
+Count</t>
+  </si>
+  <si>
+    <t>Tier 2 
+Count</t>
+  </si>
+  <si>
+    <t>Tier 3 
+Count</t>
+  </si>
+  <si>
+    <t>Tier 4 
+Count</t>
+  </si>
+  <si>
+    <t>Tier 5 
+Count</t>
+  </si>
+  <si>
+    <t>Tier
+(unassigned) 
+Count</t>
+  </si>
+  <si>
+    <t>Application Modernization</t>
+  </si>
+  <si>
+    <t>Data Modernization</t>
+  </si>
+  <si>
+    <t>Infrastructure Modernization</t>
   </si>
 </sst>
 </file>
@@ -167,7 +236,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -180,8 +249,14 @@
         <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -189,11 +264,20 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -236,6 +320,15 @@
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -637,11 +730,11 @@
       <c r="Y1" s="8"/>
     </row>
     <row r="2" spans="1:25" ht="22.5" x14ac:dyDescent="0.45">
-      <c r="A2" s="22" t="s">
+      <c r="A2" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="22"/>
-      <c r="C2" s="22"/>
+      <c r="B2" s="25"/>
+      <c r="C2" s="25"/>
       <c r="E2" s="8"/>
       <c r="F2" s="8"/>
       <c r="G2" s="8"/>
@@ -782,7 +875,7 @@
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="15.6328125" style="20" customWidth="1"/>
-    <col min="2" max="2" width="55.453125" style="20" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="58.453125" style="20" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="32.1796875" style="20" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="26.26953125" style="20" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="15.453125" style="20" bestFit="1" customWidth="1"/>
@@ -898,7 +991,7 @@
     <row r="2" spans="1:34" ht="29.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="19"/>
       <c r="B2" s="18" t="s">
-        <v>8</v>
+        <v>24</v>
       </c>
       <c r="C2" s="21"/>
       <c r="D2" s="21"/>
@@ -974,7 +1067,7 @@
         <v>1</v>
       </c>
       <c r="B4" s="20" t="s">
-        <v>8</v>
+        <v>24</v>
       </c>
     </row>
     <row r="5" spans="1:34" ht="24" x14ac:dyDescent="0.35">
@@ -1127,7 +1220,7 @@
     <row r="2" spans="1:34" ht="29.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="1"/>
       <c r="B2" s="3" t="s">
-        <v>9</v>
+        <v>25</v>
       </c>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
@@ -1203,7 +1296,7 @@
         <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>9</v>
+        <v>25</v>
       </c>
     </row>
     <row r="5" spans="1:34" ht="24" x14ac:dyDescent="0.35">
@@ -1240,7 +1333,7 @@
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="15.6328125" customWidth="1"/>
-    <col min="2" max="2" width="55.453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="63.26953125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="32.1796875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="26.26953125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="15.453125" bestFit="1" customWidth="1"/>
@@ -1355,7 +1448,7 @@
     <row r="2" spans="1:34" ht="29.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="1"/>
       <c r="B2" s="3" t="s">
-        <v>10</v>
+        <v>26</v>
       </c>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
@@ -1431,7 +1524,7 @@
         <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>10</v>
+        <v>26</v>
       </c>
     </row>
     <row r="5" spans="1:34" ht="24" x14ac:dyDescent="0.35">
@@ -1455,13 +1548,99 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E4CA8D1F-1157-4282-9791-3897C49F83F0}">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2C63458-CE14-4763-837A-3AF9856D458B}">
+  <dimension ref="A1:V1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView zoomScale="68" zoomScaleNormal="68" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="13.7265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.6328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.453125" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="12.81640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="5.6328125" customWidth="1"/>
+    <col min="8" max="12" width="12.81640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="18.54296875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="5.6328125" customWidth="1"/>
+    <col min="15" max="18" width="16.6328125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="16.36328125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="21.7265625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="19.6328125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="20.6328125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:22" s="22" customFormat="1" ht="39" x14ac:dyDescent="0.3">
+      <c r="A1" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="23" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="23" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="24" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1" s="24" t="s">
+        <v>13</v>
+      </c>
+      <c r="G1" s="24"/>
+      <c r="H1" s="24" t="s">
+        <v>18</v>
+      </c>
+      <c r="I1" s="24" t="s">
+        <v>19</v>
+      </c>
+      <c r="J1" s="24" t="s">
+        <v>20</v>
+      </c>
+      <c r="K1" s="24" t="s">
+        <v>21</v>
+      </c>
+      <c r="L1" s="24" t="s">
+        <v>22</v>
+      </c>
+      <c r="M1" s="24" t="s">
+        <v>23</v>
+      </c>
+      <c r="N1" s="24"/>
+      <c r="O1" s="24" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" s="24" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1" s="24" t="s">
+        <v>16</v>
+      </c>
+      <c r="R1" s="24" t="s">
+        <v>17</v>
+      </c>
+      <c r="S1" s="24" t="s">
+        <v>12</v>
+      </c>
+      <c r="T1" s="24" t="s">
+        <v>8</v>
+      </c>
+      <c r="U1" s="24" t="s">
+        <v>9</v>
+      </c>
+      <c r="V1" s="24" t="s">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:V1" xr:uid="{E2C63458-CE14-4763-837A-3AF9856D458B}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>